<commit_message>
updating team_table. Should have everything now
</commit_message>
<xml_diff>
--- a/data/team variables list.xlsx
+++ b/data/team variables list.xlsx
@@ -473,7 +473,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,12 +598,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>